<commit_message>
Add chapter selection and word stacking
</commit_message>
<xml_diff>
--- a/public/words.xlsx
+++ b/public/words.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="502">
   <si>
     <t>abstruse</t>
   </si>
@@ -433,25 +433,1090 @@
     <t>boisterous</t>
   </si>
   <si>
+    <t>시끄러운</t>
+  </si>
+  <si>
     <t>bombastic</t>
   </si>
   <si>
+    <t>허풍 떠는, 허세부리는</t>
+  </si>
+  <si>
     <t>brazen</t>
   </si>
   <si>
+    <t>뻔뻔한</t>
+  </si>
+  <si>
     <t>bucolic</t>
   </si>
   <si>
+    <t>전원적인</t>
+  </si>
+  <si>
     <t>calamity</t>
   </si>
   <si>
+    <t>재앙, 재난</t>
+  </si>
+  <si>
     <t>callow</t>
   </si>
   <si>
+    <t>미성숙한, 경험 없는</t>
+  </si>
+  <si>
+    <t>변덕스러운</t>
+  </si>
+  <si>
     <t>castigate</t>
   </si>
   <si>
+    <t>징계하다, 비난하다</t>
+  </si>
+  <si>
     <t>champion</t>
+  </si>
+  <si>
+    <t>옹호하다, 지지하다</t>
+  </si>
+  <si>
+    <t>chary</t>
+  </si>
+  <si>
+    <t>조심하는, 신중한, 절약하는</t>
+  </si>
+  <si>
+    <t>circumscribe</t>
+  </si>
+  <si>
+    <t>제한하다</t>
+  </si>
+  <si>
+    <t>circumspect</t>
+  </si>
+  <si>
+    <t>신중한, 주의 깊은, 조심하는</t>
+  </si>
+  <si>
+    <t>cliche</t>
+  </si>
+  <si>
+    <t>진부한 표현</t>
+  </si>
+  <si>
+    <t>commensurate</t>
+  </si>
+  <si>
+    <t>동등한, 같은, 크기의, 비례하는</t>
+  </si>
+  <si>
+    <t>compliant</t>
+  </si>
+  <si>
+    <t>순응하는, 따르는</t>
+  </si>
+  <si>
+    <t>compromise</t>
+  </si>
+  <si>
+    <t>위태롭게 하다, 훼손하다</t>
+  </si>
+  <si>
+    <t>condescend</t>
+  </si>
+  <si>
+    <t>생색내다, 오만하게 행동하다</t>
+  </si>
+  <si>
+    <t>conjecture</t>
+  </si>
+  <si>
+    <t>추정, 추측</t>
+  </si>
+  <si>
+    <t>consolidate</t>
+  </si>
+  <si>
+    <t>통합하다, 굳히다, 강화하다</t>
+  </si>
+  <si>
+    <t>conspicuous</t>
+  </si>
+  <si>
+    <t>눈에 잘 띄는, 튀는, 뚜렷한</t>
+  </si>
+  <si>
+    <t>construe</t>
+  </si>
+  <si>
+    <t>해석하다</t>
+  </si>
+  <si>
+    <t>contentious</t>
+  </si>
+  <si>
+    <t>논쟁적인, 논쟁을 일으키는</t>
+  </si>
+  <si>
+    <t>conundrum</t>
+  </si>
+  <si>
+    <t>난제, 수수께끼</t>
+  </si>
+  <si>
+    <t>convoluted</t>
+  </si>
+  <si>
+    <t>복잡한, 난해한</t>
+  </si>
+  <si>
+    <t>corroborate</t>
+  </si>
+  <si>
+    <t>확증하다</t>
+  </si>
+  <si>
+    <t>dauntless</t>
+  </si>
+  <si>
+    <t>겁 없는</t>
+  </si>
+  <si>
+    <t>debilitate</t>
+  </si>
+  <si>
+    <t>쇠약하게 만들다</t>
+  </si>
+  <si>
+    <t>decorous</t>
+  </si>
+  <si>
+    <t>단정한, 예의 바른</t>
+  </si>
+  <si>
+    <t>decry</t>
+  </si>
+  <si>
+    <t>비난하다</t>
+  </si>
+  <si>
+    <t>deference</t>
+  </si>
+  <si>
+    <t>존중</t>
+  </si>
+  <si>
+    <t>defiant</t>
+  </si>
+  <si>
+    <t>반항하는</t>
+  </si>
+  <si>
+    <t>deject</t>
+  </si>
+  <si>
+    <t>사기를 꺾다, 낙담시키다</t>
+  </si>
+  <si>
+    <t>deleterious</t>
+  </si>
+  <si>
+    <t>해로운</t>
+  </si>
+  <si>
+    <t>deliberate</t>
+  </si>
+  <si>
+    <t>(v)숙고하다 (adj)신중한, 고의의</t>
+  </si>
+  <si>
+    <t>derogatory</t>
+  </si>
+  <si>
+    <t>격하시키는, 폄하하는</t>
+  </si>
+  <si>
+    <t>detractor</t>
+  </si>
+  <si>
+    <t>가치를 깎아내리는 사람</t>
+  </si>
+  <si>
+    <t>digress</t>
+  </si>
+  <si>
+    <t>벗어나다</t>
+  </si>
+  <si>
+    <t>dire</t>
+  </si>
+  <si>
+    <t>끔찍한, 비참한, 절박한, 엄청난</t>
+  </si>
+  <si>
+    <t>desciplined</t>
+  </si>
+  <si>
+    <t>기강을 따르는, 훈련된, 단련된</t>
+  </si>
+  <si>
+    <t>discredit</t>
+  </si>
+  <si>
+    <t>존경심을 떨어뜨리다, 신빙성을 없애다</t>
+  </si>
+  <si>
+    <t>discriminating</t>
+  </si>
+  <si>
+    <t>식별력 있는, 안목이 있는</t>
+  </si>
+  <si>
+    <t>disparage</t>
+  </si>
+  <si>
+    <t>깎아내리다, 폄하하다</t>
+  </si>
+  <si>
+    <t>dissemble</t>
+  </si>
+  <si>
+    <t>숨기다, 가식적으로 꾸미다, 가장하다</t>
+  </si>
+  <si>
+    <t>divulge</t>
+  </si>
+  <si>
+    <t>누설하다, 알리다</t>
+  </si>
+  <si>
+    <t>dogmatic</t>
+  </si>
+  <si>
+    <t>독단적인</t>
+  </si>
+  <si>
+    <t>doldrums</t>
+  </si>
+  <si>
+    <t>침체기, 부진, 침울, 우울</t>
+  </si>
+  <si>
+    <t>duplicity</t>
+  </si>
+  <si>
+    <t>이중성, 표리부동</t>
+  </si>
+  <si>
+    <t>ebullient</t>
+  </si>
+  <si>
+    <t>활기/열정이 넘치는, 패기 넘치는, 비등하는</t>
+  </si>
+  <si>
+    <t>eccentric</t>
+  </si>
+  <si>
+    <t>별난, 엉뚱한</t>
+  </si>
+  <si>
+    <t>eclectic</t>
+  </si>
+  <si>
+    <t>다양한, 다방면의</t>
+  </si>
+  <si>
+    <t>egalitarian</t>
+  </si>
+  <si>
+    <t>평등주의적인</t>
+  </si>
+  <si>
+    <t>embellish</t>
+  </si>
+  <si>
+    <t>꾸미다, 장식하다</t>
+  </si>
+  <si>
+    <t>encomium</t>
+  </si>
+  <si>
+    <t>찬사</t>
+  </si>
+  <si>
+    <t>engaging</t>
+  </si>
+  <si>
+    <t>호감이 가는, 매력적인</t>
+  </si>
+  <si>
+    <t>engender</t>
+  </si>
+  <si>
+    <t>낳다, 일으키다</t>
+  </si>
+  <si>
+    <t>enmity</t>
+  </si>
+  <si>
+    <t>적대감</t>
+  </si>
+  <si>
+    <t>ephemeral</t>
+  </si>
+  <si>
+    <t>일시적인, 덧없는</t>
+  </si>
+  <si>
+    <t>epitomize</t>
+  </si>
+  <si>
+    <t>요약하다, 전형이 되다</t>
+  </si>
+  <si>
+    <t>equable</t>
+  </si>
+  <si>
+    <t>차분한, 기온 변화가 적은, 고른</t>
+  </si>
+  <si>
+    <t>equitable</t>
+  </si>
+  <si>
+    <t>공평한, 공정한</t>
+  </si>
+  <si>
+    <t>erratic</t>
+  </si>
+  <si>
+    <t>불규칙한, 변덕스러운</t>
+  </si>
+  <si>
+    <t>estimable</t>
+  </si>
+  <si>
+    <t>존경할 만한, 어림(평가)할 수 있는</t>
+  </si>
+  <si>
+    <t>exalt</t>
+  </si>
+  <si>
+    <t>높이다, 칭송하다</t>
+  </si>
+  <si>
+    <t>exhaustive</t>
+  </si>
+  <si>
+    <t>포괄적인, 철저한</t>
+  </si>
+  <si>
+    <t>expedient</t>
+  </si>
+  <si>
+    <t>편의주의적인, 편리한</t>
+  </si>
+  <si>
+    <t>expeditious</t>
+  </si>
+  <si>
+    <t>신속한</t>
+  </si>
+  <si>
+    <t>extricate</t>
+  </si>
+  <si>
+    <t>(위험에서)벗어나게 하다</t>
+  </si>
+  <si>
+    <t>exultant</t>
+  </si>
+  <si>
+    <t>매우 기뻐하는</t>
+  </si>
+  <si>
+    <t>fastidious</t>
+  </si>
+  <si>
+    <t>꼼꼼한, 까다로운</t>
+  </si>
+  <si>
+    <t>fatuous</t>
+  </si>
+  <si>
+    <t>어리석은, 바보같은</t>
+  </si>
+  <si>
+    <t>feckless</t>
+  </si>
+  <si>
+    <t>쓸모없는, 무책임한</t>
+  </si>
+  <si>
+    <t>fervent</t>
+  </si>
+  <si>
+    <t>열렬한</t>
+  </si>
+  <si>
+    <t>fitful</t>
+  </si>
+  <si>
+    <t>불규칙적인, 발작적인</t>
+  </si>
+  <si>
+    <t>flamboyant</t>
+  </si>
+  <si>
+    <t>눈부신, 화려한, 현란한</t>
+  </si>
+  <si>
+    <t>flippant</t>
+  </si>
+  <si>
+    <t>경박한, 성의없는(가볍고 무례한)</t>
+  </si>
+  <si>
+    <t>forestall</t>
+  </si>
+  <si>
+    <t>미연에 방지하다, 기선을 제압하다</t>
+  </si>
+  <si>
+    <t>formidable</t>
+  </si>
+  <si>
+    <t>겁먹게 하는, 위협적인, 경외감을 갖게 하는</t>
+  </si>
+  <si>
+    <t>forswear</t>
+  </si>
+  <si>
+    <t>포기하다, 위증하다</t>
+  </si>
+  <si>
+    <t>fortuitous</t>
+  </si>
+  <si>
+    <t>우연한</t>
+  </si>
+  <si>
+    <t>fractious</t>
+  </si>
+  <si>
+    <t>화/짜증을 잘 내는, 다루기 힘든</t>
+  </si>
+  <si>
+    <t>frivolous</t>
+  </si>
+  <si>
+    <t>가벼운, 경박한, 하찮은</t>
+  </si>
+  <si>
+    <t>frugal</t>
+  </si>
+  <si>
+    <t>절약하는</t>
+  </si>
+  <si>
+    <t>fulmination</t>
+  </si>
+  <si>
+    <t>심한 비난</t>
+  </si>
+  <si>
+    <t>gainsay</t>
+  </si>
+  <si>
+    <t>반박하다, 부인하다, 반대하다</t>
+  </si>
+  <si>
+    <t>glib</t>
+  </si>
+  <si>
+    <t>말만 유창한, 입심좋은</t>
+  </si>
+  <si>
+    <t>gossamer</t>
+  </si>
+  <si>
+    <t>매우 얇은, 섬세한</t>
+  </si>
+  <si>
+    <t>grandiloquent</t>
+  </si>
+  <si>
+    <t>과장된, 허풍떠는</t>
+  </si>
+  <si>
+    <t>gratuitous</t>
+  </si>
+  <si>
+    <t>무료의, 필요없는, 근거없는</t>
+  </si>
+  <si>
+    <t>gritty</t>
+  </si>
+  <si>
+    <t>용감한, 단호한</t>
+  </si>
+  <si>
+    <t>hamstring</t>
+  </si>
+  <si>
+    <t>무력화하다, 좌절시키다, 방해하다</t>
+  </si>
+  <si>
+    <t>haphazard</t>
+  </si>
+  <si>
+    <t>아무렇게나, 되는대로</t>
+  </si>
+  <si>
+    <t>harangue</t>
+  </si>
+  <si>
+    <t>(v)열변을 토하다 (n)비난, 질책</t>
+  </si>
+  <si>
+    <t>hardheaded</t>
+  </si>
+  <si>
+    <t>완고한, 현실적인, 빈틈없는, 냉정한</t>
+  </si>
+  <si>
+    <t>hauteur</t>
+  </si>
+  <si>
+    <t>오만함, 거만한 태도</t>
+  </si>
+  <si>
+    <t>hedonism</t>
+  </si>
+  <si>
+    <t>쾌락주의</t>
+  </si>
+  <si>
+    <t>hobnob</t>
+  </si>
+  <si>
+    <t>친하게 지내다, 사귀다</t>
+  </si>
+  <si>
+    <t>hodgepodge</t>
+  </si>
+  <si>
+    <t>뒤범벅, 잡탕</t>
+  </si>
+  <si>
+    <t>hone</t>
+  </si>
+  <si>
+    <t>(v)날카롭게 하다 (n)숫돌</t>
+  </si>
+  <si>
+    <t>humdrum</t>
+  </si>
+  <si>
+    <t>단조로운, 재미없는</t>
+  </si>
+  <si>
+    <t>husband</t>
+  </si>
+  <si>
+    <t>절약하다</t>
+  </si>
+  <si>
+    <t>idyllic</t>
+  </si>
+  <si>
+    <t>목가적인</t>
+  </si>
+  <si>
+    <t>impassionate</t>
+  </si>
+  <si>
+    <t>열정적인</t>
+  </si>
+  <si>
+    <t>impecunious</t>
+  </si>
+  <si>
+    <t>무일푼의</t>
+  </si>
+  <si>
+    <t>imperious</t>
+  </si>
+  <si>
+    <t>오만한, 고압적인</t>
+  </si>
+  <si>
+    <t>impetuous</t>
+  </si>
+  <si>
+    <t>충동적인, 성급한</t>
+  </si>
+  <si>
+    <t>inane</t>
+  </si>
+  <si>
+    <t>무의미한, 어리석은</t>
+  </si>
+  <si>
+    <t>incisive</t>
+  </si>
+  <si>
+    <t>예리한, 날카로운, 통렬한</t>
+  </si>
+  <si>
+    <t>inclement</t>
+  </si>
+  <si>
+    <t>(날씨가)혹독한, 궂은</t>
+  </si>
+  <si>
+    <t>incorporate</t>
+  </si>
+  <si>
+    <t>포함하다, 통합시키다</t>
+  </si>
+  <si>
+    <t>indigent</t>
+  </si>
+  <si>
+    <t>궁핍한, (생필품이)결핍된</t>
+  </si>
+  <si>
+    <t>indolent</t>
+  </si>
+  <si>
+    <t>게으른</t>
+  </si>
+  <si>
+    <t>inexorable</t>
+  </si>
+  <si>
+    <t>설득할 수 없는, 무자비한, 가차없는, 냉혹한</t>
+  </si>
+  <si>
+    <t>inimical</t>
+  </si>
+  <si>
+    <t>해로운, 적대적인</t>
+  </si>
+  <si>
+    <t>innocuous</t>
+  </si>
+  <si>
+    <t>무해한</t>
+  </si>
+  <si>
+    <t>innuendo</t>
+  </si>
+  <si>
+    <t>넌지시 비침, 빗댐, 암시</t>
+  </si>
+  <si>
+    <t>insolent</t>
+  </si>
+  <si>
+    <t>무례한, 불손한</t>
+  </si>
+  <si>
+    <t>insular</t>
+  </si>
+  <si>
+    <t>배타적인, 편협한</t>
+  </si>
+  <si>
+    <t>integrity</t>
+  </si>
+  <si>
+    <t>1. 정직, 청렴 2. 완전한 상태, 온전함, 보전</t>
+  </si>
+  <si>
+    <t>넌지시 알려주다, 암시하다</t>
+  </si>
+  <si>
+    <t>intransigent</t>
+  </si>
+  <si>
+    <t>비타협적인, 완고한</t>
+  </si>
+  <si>
+    <t>intrepid</t>
+  </si>
+  <si>
+    <t>겁 없는, 대담한</t>
+  </si>
+  <si>
+    <t>jaded</t>
+  </si>
+  <si>
+    <t>지긋지긋한, 싫증난</t>
+  </si>
+  <si>
+    <t>jaundiced</t>
+  </si>
+  <si>
+    <t>편견을 가진</t>
+  </si>
+  <si>
+    <t>laconic</t>
+  </si>
+  <si>
+    <t>간결한, 과묵한</t>
+  </si>
+  <si>
+    <t>lassitude</t>
+  </si>
+  <si>
+    <t>무기력</t>
+  </si>
+  <si>
+    <t>laud</t>
+  </si>
+  <si>
+    <t>칭찬하다, 찬양하다</t>
+  </si>
+  <si>
+    <t>lenient</t>
+  </si>
+  <si>
+    <t>(처벌/규칙 적용이)관대한</t>
+  </si>
+  <si>
+    <t>lionize</t>
+  </si>
+  <si>
+    <t>명사로 대접해주다, 치켜세우다</t>
+  </si>
+  <si>
+    <t>loath</t>
+  </si>
+  <si>
+    <t>내켜 하지 않는, 꺼리는</t>
+  </si>
+  <si>
+    <t>loquacious</t>
+  </si>
+  <si>
+    <t>매우 수다스러운</t>
+  </si>
+  <si>
+    <t>lucid</t>
+  </si>
+  <si>
+    <t>맑고 투명한, 명료한, 명쾌한</t>
+  </si>
+  <si>
+    <t>lugubrious</t>
+  </si>
+  <si>
+    <t>침울한, 슬픈</t>
+  </si>
+  <si>
+    <t>maladroit</t>
+  </si>
+  <si>
+    <t>솜씨없는, 서투른</t>
+  </si>
+  <si>
+    <t>malleable</t>
+  </si>
+  <si>
+    <t>(금속)변형이 잘 되는</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>망치다, 손상시키다</t>
+  </si>
+  <si>
+    <t>maverick</t>
+  </si>
+  <si>
+    <t>독불장군</t>
+  </si>
+  <si>
+    <t>mediocre</t>
+  </si>
+  <si>
+    <t>보통밖에 안 되는, 썩 좋지는 않은</t>
+  </si>
+  <si>
+    <t>mellifluous</t>
+  </si>
+  <si>
+    <t>(소리/말이)감미로운</t>
+  </si>
+  <si>
+    <t>mendacious</t>
+  </si>
+  <si>
+    <t>진실을 말하지 않는, 허위인</t>
+  </si>
+  <si>
+    <t>mercurial</t>
+  </si>
+  <si>
+    <t>매우 꼼꼼한, 주의 깊은, 정확한</t>
+  </si>
+  <si>
+    <t>miser</t>
+  </si>
+  <si>
+    <t>구두쇠</t>
+  </si>
+  <si>
+    <t>mordant</t>
+  </si>
+  <si>
+    <t>신랄한, 통렬한</t>
+  </si>
+  <si>
+    <t>mundane</t>
+  </si>
+  <si>
+    <t>평범한, 흔한, 재미없는, 일상적인</t>
+  </si>
+  <si>
+    <t>nadir</t>
+  </si>
+  <si>
+    <t>밑바닥, 절망상태</t>
+  </si>
+  <si>
+    <t>natty</t>
+  </si>
+  <si>
+    <t>말끔한</t>
+  </si>
+  <si>
+    <t>nettle</t>
+  </si>
+  <si>
+    <t>화나게 하다, 안절부절 못하게하다</t>
+  </si>
+  <si>
+    <t>nonchalant</t>
+  </si>
+  <si>
+    <t>걱정근심 없는, 무사태평한, 무심한, 태연한</t>
+  </si>
+  <si>
+    <t>nugatory</t>
+  </si>
+  <si>
+    <t>중요하지 않은, 하찮은</t>
+  </si>
+  <si>
+    <t>obdurate</t>
+  </si>
+  <si>
+    <t>고집 센</t>
+  </si>
+  <si>
+    <t>obfuscate</t>
+  </si>
+  <si>
+    <t>혼란스럽게 만들다</t>
+  </si>
+  <si>
+    <t>oblivious</t>
+  </si>
+  <si>
+    <t>알아채지 못한, 염두에 없는, 망각한</t>
+  </si>
+  <si>
+    <t>obviate</t>
+  </si>
+  <si>
+    <t>미리 막다, 피하다</t>
+  </si>
+  <si>
+    <t>onerous</t>
+  </si>
+  <si>
+    <t>힘든, 성가신, 귀찮은</t>
+  </si>
+  <si>
+    <t>opaque</t>
+  </si>
+  <si>
+    <t>불투명한, 불분명한, 이해하기 힘든</t>
+  </si>
+  <si>
+    <t>opprobrium</t>
+  </si>
+  <si>
+    <t>불명예, 비난</t>
+  </si>
+  <si>
+    <t>orthodox</t>
+  </si>
+  <si>
+    <t>정설의, 정교의</t>
+  </si>
+  <si>
+    <t>oscillate</t>
+  </si>
+  <si>
+    <t>진동하다, 주저하다, 흔들리다</t>
+  </si>
+  <si>
+    <t>ostentatious</t>
+  </si>
+  <si>
+    <t>자랑/과시하는, 허세부리는</t>
+  </si>
+  <si>
+    <t>painstaking</t>
+  </si>
+  <si>
+    <t>애쓰는, 수고를 아끼지 않는, 면밀한, 철저한</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>심하게 비난하다</t>
+  </si>
+  <si>
+    <t>panacea</t>
+  </si>
+  <si>
+    <t>만병통치약</t>
+  </si>
+  <si>
+    <t>paradigm</t>
+  </si>
+  <si>
+    <t>전형적인 예</t>
+  </si>
+  <si>
+    <t>partisan</t>
+  </si>
+  <si>
+    <t>(n)열렬한 지지자 (a)편파적인</t>
+  </si>
+  <si>
+    <t>prosaic</t>
+  </si>
+  <si>
+    <t>진부한, 재미없는, 지겨운</t>
+  </si>
+  <si>
+    <t>pugnacious</t>
+  </si>
+  <si>
+    <t>호전적인</t>
+  </si>
+  <si>
+    <t>recant</t>
+  </si>
+  <si>
+    <t>(주장)철회하다, (신념)부정하다</t>
+  </si>
+  <si>
+    <t>reconcile</t>
+  </si>
+  <si>
+    <t>화해시키다, 조화롭게 하다</t>
+  </si>
+  <si>
+    <t>repudiate</t>
+  </si>
+  <si>
+    <t>부인하다, 거절하다</t>
+  </si>
+  <si>
+    <t>revile</t>
+  </si>
+  <si>
+    <t>rudimentary</t>
+  </si>
+  <si>
+    <t>미성숙의, 기본적인</t>
+  </si>
+  <si>
+    <t>salubrious</t>
+  </si>
+  <si>
+    <t>건강에 좋은, 유익한, 건강한</t>
+  </si>
+  <si>
+    <t>shore up</t>
+  </si>
+  <si>
+    <t>지탱하다, 떠받치다</t>
+  </si>
+  <si>
+    <t>subvert</t>
+  </si>
+  <si>
+    <t>(권력/시스템을)약화시키다</t>
+  </si>
+  <si>
+    <t>tendentious</t>
+  </si>
+  <si>
+    <t>편향적인</t>
+  </si>
+  <si>
+    <t>tractable</t>
+  </si>
+  <si>
+    <t>다루기 쉬운, 유순한</t>
+  </si>
+  <si>
+    <t>trepidation</t>
+  </si>
+  <si>
+    <t>두려움</t>
+  </si>
+  <si>
+    <t>temporal</t>
+  </si>
+  <si>
+    <t>현세의, 속세의</t>
+  </si>
+  <si>
+    <t>unseemly</t>
+  </si>
+  <si>
+    <t>(행동이)적절하지 않은</t>
+  </si>
+  <si>
+    <t>urbane</t>
+  </si>
+  <si>
+    <t>(특히 남자가)세련되고 친절한, 교양있는</t>
+  </si>
+  <si>
+    <t>vagary</t>
+  </si>
+  <si>
+    <t>변덕, 엉뚱한 짓</t>
+  </si>
+  <si>
+    <t>vainglorious</t>
+  </si>
+  <si>
+    <t>허영심이 강한</t>
+  </si>
+  <si>
+    <t>vivacious</t>
+  </si>
+  <si>
+    <t>(특히 여성)쾌활한, 명랑한, 생기 넘치는</t>
+  </si>
+  <si>
+    <t>wane</t>
+  </si>
+  <si>
+    <t>작아지다, 약해지다, 달이 기울다</t>
   </si>
 </sst>
 </file>
@@ -468,7 +1533,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -490,15 +1554,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,6 +1803,12 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -750,6 +1826,11 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -770,6 +1851,10 @@
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -790,6 +1875,10 @@
       <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -810,6 +1899,10 @@
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -859,6 +1952,11 @@
       <c r="E7" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
@@ -873,6 +1971,12 @@
       <c r="D8" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -890,12 +1994,17 @@
       <c r="E9" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -913,6 +2022,9 @@
       <c r="G10" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -933,6 +2045,10 @@
       <c r="F11" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
@@ -941,6 +2057,14 @@
       <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
@@ -955,6 +2079,12 @@
       <c r="D13" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
@@ -969,6 +2099,12 @@
       <c r="D14" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
@@ -983,6 +2119,12 @@
       <c r="D15" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
@@ -1009,6 +2151,8 @@
       <c r="H16" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
@@ -1029,6 +2173,10 @@
       <c r="F17" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
@@ -1058,6 +2206,7 @@
       <c r="I18" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="J18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
@@ -1066,14 +2215,30 @@
       <c r="B19" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
@@ -1082,6 +2247,14 @@
       <c r="B21" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
@@ -1090,6 +2263,14 @@
       <c r="B22" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
@@ -1107,6 +2288,11 @@
       <c r="E23" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
@@ -1124,6 +2310,11 @@
       <c r="E24" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
@@ -1135,6 +2326,13 @@
       <c r="C25" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
@@ -1149,6 +2347,12 @@
       <c r="D26" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
@@ -1166,6 +2370,11 @@
       <c r="E27" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
@@ -1186,12 +2395,16 @@
       <c r="F28" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>135</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1203,51 +2416,2971 @@
       <c r="E29" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="B30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>140</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>143</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="B36" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A38" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="2"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+      <c r="J127" s="2"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+      <c r="J129" s="2"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C130" s="2"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+      <c r="J130" s="2"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+      <c r="J131" s="2"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+      <c r="H132" s="2"/>
+      <c r="I132" s="2"/>
+      <c r="J132" s="2"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C133" s="2"/>
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+      <c r="J133" s="2"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+      <c r="J134" s="2"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="2"/>
+      <c r="I135" s="2"/>
+      <c r="J135" s="2"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+      <c r="J136" s="2"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+      <c r="J137" s="2"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+      <c r="J138" s="2"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+      <c r="J139" s="2"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+      <c r="J141" s="2"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+      <c r="H143" s="2"/>
+      <c r="I143" s="2"/>
+      <c r="J143" s="2"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+      <c r="J144" s="2"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+      <c r="J145" s="2"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+      <c r="J147" s="2"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+      <c r="J148" s="2"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+      <c r="H149" s="2"/>
+      <c r="I149" s="2"/>
+      <c r="J149" s="2"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+      <c r="H150" s="2"/>
+      <c r="I150" s="2"/>
+      <c r="J150" s="2"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+      <c r="H151" s="2"/>
+      <c r="I151" s="2"/>
+      <c r="J151" s="2"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+      <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+      <c r="J152" s="2"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2"/>
+      <c r="H153" s="2"/>
+      <c r="I153" s="2"/>
+      <c r="J153" s="2"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+      <c r="J155" s="2"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C156" s="2"/>
+      <c r="D156" s="2"/>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+      <c r="H156" s="2"/>
+      <c r="I156" s="2"/>
+      <c r="J156" s="2"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+      <c r="H157" s="2"/>
+      <c r="I157" s="2"/>
+      <c r="J157" s="2"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+      <c r="H158" s="2"/>
+      <c r="I158" s="2"/>
+      <c r="J158" s="2"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2"/>
+      <c r="H159" s="2"/>
+      <c r="I159" s="2"/>
+      <c r="J159" s="2"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
+      <c r="J161" s="2"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="2"/>
+      <c r="H162" s="2"/>
+      <c r="I162" s="2"/>
+      <c r="J162" s="2"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="2"/>
+      <c r="H163" s="2"/>
+      <c r="I163" s="2"/>
+      <c r="J163" s="2"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2"/>
+      <c r="H164" s="2"/>
+      <c r="I164" s="2"/>
+      <c r="J164" s="2"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
+      <c r="J165" s="2"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+      <c r="H166" s="2"/>
+      <c r="I166" s="2"/>
+      <c r="J166" s="2"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C167" s="2"/>
+      <c r="D167" s="2"/>
+      <c r="E167" s="2"/>
+      <c r="F167" s="2"/>
+      <c r="G167" s="2"/>
+      <c r="H167" s="2"/>
+      <c r="I167" s="2"/>
+      <c r="J167" s="2"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
+      <c r="G168" s="2"/>
+      <c r="H168" s="2"/>
+      <c r="I168" s="2"/>
+      <c r="J168" s="2"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="2"/>
+      <c r="H169" s="2"/>
+      <c r="I169" s="2"/>
+      <c r="J169" s="2"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="2"/>
+      <c r="H170" s="2"/>
+      <c r="I170" s="2"/>
+      <c r="J170" s="2"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C171" s="2"/>
+      <c r="D171" s="2"/>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
+      <c r="G171" s="2"/>
+      <c r="H171" s="2"/>
+      <c r="I171" s="2"/>
+      <c r="J171" s="2"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C172" s="2"/>
+      <c r="D172" s="2"/>
+      <c r="E172" s="2"/>
+      <c r="F172" s="2"/>
+      <c r="G172" s="2"/>
+      <c r="H172" s="2"/>
+      <c r="I172" s="2"/>
+      <c r="J172" s="2"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C173" s="2"/>
+      <c r="D173" s="2"/>
+      <c r="E173" s="2"/>
+      <c r="F173" s="2"/>
+      <c r="G173" s="2"/>
+      <c r="H173" s="2"/>
+      <c r="I173" s="2"/>
+      <c r="J173" s="2"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C174" s="2"/>
+      <c r="D174" s="2"/>
+      <c r="E174" s="2"/>
+      <c r="F174" s="2"/>
+      <c r="G174" s="2"/>
+      <c r="H174" s="2"/>
+      <c r="I174" s="2"/>
+      <c r="J174" s="2"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
+      <c r="E175" s="2"/>
+      <c r="F175" s="2"/>
+      <c r="G175" s="2"/>
+      <c r="H175" s="2"/>
+      <c r="I175" s="2"/>
+      <c r="J175" s="2"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
+      <c r="E176" s="2"/>
+      <c r="F176" s="2"/>
+      <c r="G176" s="2"/>
+      <c r="H176" s="2"/>
+      <c r="I176" s="2"/>
+      <c r="J176" s="2"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C177" s="2"/>
+      <c r="D177" s="2"/>
+      <c r="E177" s="2"/>
+      <c r="F177" s="2"/>
+      <c r="G177" s="2"/>
+      <c r="H177" s="2"/>
+      <c r="I177" s="2"/>
+      <c r="J177" s="2"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="2"/>
+      <c r="F178" s="2"/>
+      <c r="G178" s="2"/>
+      <c r="H178" s="2"/>
+      <c r="I178" s="2"/>
+      <c r="J178" s="2"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
+      <c r="E179" s="2"/>
+      <c r="F179" s="2"/>
+      <c r="G179" s="2"/>
+      <c r="H179" s="2"/>
+      <c r="I179" s="2"/>
+      <c r="J179" s="2"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="2"/>
+      <c r="F180" s="2"/>
+      <c r="G180" s="2"/>
+      <c r="H180" s="2"/>
+      <c r="I180" s="2"/>
+      <c r="J180" s="2"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="2"/>
+      <c r="F181" s="2"/>
+      <c r="G181" s="2"/>
+      <c r="H181" s="2"/>
+      <c r="I181" s="2"/>
+      <c r="J181" s="2"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
+      <c r="E182" s="2"/>
+      <c r="F182" s="2"/>
+      <c r="G182" s="2"/>
+      <c r="H182" s="2"/>
+      <c r="I182" s="2"/>
+      <c r="J182" s="2"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C183" s="2"/>
+      <c r="D183" s="2"/>
+      <c r="E183" s="2"/>
+      <c r="F183" s="2"/>
+      <c r="G183" s="2"/>
+      <c r="H183" s="2"/>
+      <c r="I183" s="2"/>
+      <c r="J183" s="2"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
+      <c r="E184" s="2"/>
+      <c r="F184" s="2"/>
+      <c r="G184" s="2"/>
+      <c r="H184" s="2"/>
+      <c r="I184" s="2"/>
+      <c r="J184" s="2"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
+      <c r="E185" s="2"/>
+      <c r="F185" s="2"/>
+      <c r="G185" s="2"/>
+      <c r="H185" s="2"/>
+      <c r="I185" s="2"/>
+      <c r="J185" s="2"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
+      <c r="E186" s="2"/>
+      <c r="F186" s="2"/>
+      <c r="G186" s="2"/>
+      <c r="H186" s="2"/>
+      <c r="I186" s="2"/>
+      <c r="J186" s="2"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C187" s="2"/>
+      <c r="D187" s="2"/>
+      <c r="E187" s="2"/>
+      <c r="F187" s="2"/>
+      <c r="G187" s="2"/>
+      <c r="H187" s="2"/>
+      <c r="I187" s="2"/>
+      <c r="J187" s="2"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C188" s="2"/>
+      <c r="D188" s="2"/>
+      <c r="E188" s="2"/>
+      <c r="F188" s="2"/>
+      <c r="G188" s="2"/>
+      <c r="H188" s="2"/>
+      <c r="I188" s="2"/>
+      <c r="J188" s="2"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C189" s="2"/>
+      <c r="D189" s="2"/>
+      <c r="E189" s="2"/>
+      <c r="F189" s="2"/>
+      <c r="G189" s="2"/>
+      <c r="H189" s="2"/>
+      <c r="I189" s="2"/>
+      <c r="J189" s="2"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C190" s="2"/>
+      <c r="D190" s="2"/>
+      <c r="E190" s="2"/>
+      <c r="F190" s="2"/>
+      <c r="G190" s="2"/>
+      <c r="H190" s="2"/>
+      <c r="I190" s="2"/>
+      <c r="J190" s="2"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C191" s="2"/>
+      <c r="D191" s="2"/>
+      <c r="E191" s="2"/>
+      <c r="F191" s="2"/>
+      <c r="G191" s="2"/>
+      <c r="H191" s="2"/>
+      <c r="I191" s="2"/>
+      <c r="J191" s="2"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C192" s="2"/>
+      <c r="D192" s="2"/>
+      <c r="E192" s="2"/>
+      <c r="F192" s="2"/>
+      <c r="G192" s="2"/>
+      <c r="H192" s="2"/>
+      <c r="I192" s="2"/>
+      <c r="J192" s="2"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C193" s="2"/>
+      <c r="D193" s="2"/>
+      <c r="E193" s="2"/>
+      <c r="F193" s="2"/>
+      <c r="G193" s="2"/>
+      <c r="H193" s="2"/>
+      <c r="I193" s="2"/>
+      <c r="J193" s="2"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="C194" s="2"/>
+      <c r="D194" s="2"/>
+      <c r="E194" s="2"/>
+      <c r="F194" s="2"/>
+      <c r="G194" s="2"/>
+      <c r="H194" s="2"/>
+      <c r="I194" s="2"/>
+      <c r="J194" s="2"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C195" s="2"/>
+      <c r="D195" s="2"/>
+      <c r="E195" s="2"/>
+      <c r="F195" s="2"/>
+      <c r="G195" s="2"/>
+      <c r="H195" s="2"/>
+      <c r="I195" s="2"/>
+      <c r="J195" s="2"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C196" s="2"/>
+      <c r="D196" s="2"/>
+      <c r="E196" s="2"/>
+      <c r="F196" s="2"/>
+      <c r="G196" s="2"/>
+      <c r="H196" s="2"/>
+      <c r="I196" s="2"/>
+      <c r="J196" s="2"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C197" s="2"/>
+      <c r="D197" s="2"/>
+      <c r="E197" s="2"/>
+      <c r="F197" s="2"/>
+      <c r="G197" s="2"/>
+      <c r="H197" s="2"/>
+      <c r="I197" s="2"/>
+      <c r="J197" s="2"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C198" s="2"/>
+      <c r="D198" s="2"/>
+      <c r="E198" s="2"/>
+      <c r="F198" s="2"/>
+      <c r="G198" s="2"/>
+      <c r="H198" s="2"/>
+      <c r="I198" s="2"/>
+      <c r="J198" s="2"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C199" s="2"/>
+      <c r="D199" s="2"/>
+      <c r="E199" s="2"/>
+      <c r="F199" s="2"/>
+      <c r="G199" s="2"/>
+      <c r="H199" s="2"/>
+      <c r="I199" s="2"/>
+      <c r="J199" s="2"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C200" s="2"/>
+      <c r="D200" s="2"/>
+      <c r="E200" s="2"/>
+      <c r="F200" s="2"/>
+      <c r="G200" s="2"/>
+      <c r="H200" s="2"/>
+      <c r="I200" s="2"/>
+      <c r="J200" s="2"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C201" s="2"/>
+      <c r="D201" s="2"/>
+      <c r="E201" s="2"/>
+      <c r="F201" s="2"/>
+      <c r="G201" s="2"/>
+      <c r="H201" s="2"/>
+      <c r="I201" s="2"/>
+      <c r="J201" s="2"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C202" s="2"/>
+      <c r="D202" s="2"/>
+      <c r="E202" s="2"/>
+      <c r="F202" s="2"/>
+      <c r="G202" s="2"/>
+      <c r="H202" s="2"/>
+      <c r="I202" s="2"/>
+      <c r="J202" s="2"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C203" s="2"/>
+      <c r="D203" s="2"/>
+      <c r="E203" s="2"/>
+      <c r="F203" s="2"/>
+      <c r="G203" s="2"/>
+      <c r="H203" s="2"/>
+      <c r="I203" s="2"/>
+      <c r="J203" s="2"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="C204" s="2"/>
+      <c r="D204" s="2"/>
+      <c r="E204" s="2"/>
+      <c r="F204" s="2"/>
+      <c r="G204" s="2"/>
+      <c r="H204" s="2"/>
+      <c r="I204" s="2"/>
+      <c r="J204" s="2"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C205" s="2"/>
+      <c r="D205" s="2"/>
+      <c r="E205" s="2"/>
+      <c r="F205" s="2"/>
+      <c r="G205" s="2"/>
+      <c r="H205" s="2"/>
+      <c r="I205" s="2"/>
+      <c r="J205" s="2"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C206" s="2"/>
+      <c r="D206" s="2"/>
+      <c r="E206" s="2"/>
+      <c r="F206" s="2"/>
+      <c r="G206" s="2"/>
+      <c r="H206" s="2"/>
+      <c r="I206" s="2"/>
+      <c r="J206" s="2"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C207" s="2"/>
+      <c r="D207" s="2"/>
+      <c r="E207" s="2"/>
+      <c r="F207" s="2"/>
+      <c r="G207" s="2"/>
+      <c r="H207" s="2"/>
+      <c r="I207" s="2"/>
+      <c r="J207" s="2"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C208" s="2"/>
+      <c r="D208" s="2"/>
+      <c r="E208" s="2"/>
+      <c r="F208" s="2"/>
+      <c r="G208" s="2"/>
+      <c r="H208" s="2"/>
+      <c r="I208" s="2"/>
+      <c r="J208" s="2"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C209" s="2"/>
+      <c r="D209" s="2"/>
+      <c r="E209" s="2"/>
+      <c r="F209" s="2"/>
+      <c r="G209" s="2"/>
+      <c r="H209" s="2"/>
+      <c r="I209" s="2"/>
+      <c r="J209" s="2"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C210" s="2"/>
+      <c r="D210" s="2"/>
+      <c r="E210" s="2"/>
+      <c r="F210" s="2"/>
+      <c r="G210" s="2"/>
+      <c r="H210" s="2"/>
+      <c r="I210" s="2"/>
+      <c r="J210" s="2"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C211" s="2"/>
+      <c r="D211" s="2"/>
+      <c r="E211" s="2"/>
+      <c r="F211" s="2"/>
+      <c r="G211" s="2"/>
+      <c r="H211" s="2"/>
+      <c r="I211" s="2"/>
+      <c r="J211" s="2"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
+      <c r="E212" s="2"/>
+      <c r="F212" s="2"/>
+      <c r="G212" s="2"/>
+      <c r="H212" s="2"/>
+      <c r="I212" s="2"/>
+      <c r="J212" s="2"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C213" s="2"/>
+      <c r="D213" s="2"/>
+      <c r="E213" s="2"/>
+      <c r="F213" s="2"/>
+      <c r="G213" s="2"/>
+      <c r="H213" s="2"/>
+      <c r="I213" s="2"/>
+      <c r="J213" s="2"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="C214" s="2"/>
+      <c r="D214" s="2"/>
+      <c r="E214" s="2"/>
+      <c r="F214" s="2"/>
+      <c r="G214" s="2"/>
+      <c r="H214" s="2"/>
+      <c r="I214" s="2"/>
+      <c r="J214" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>